<commit_message>
add package and create Test files
</commit_message>
<xml_diff>
--- a/temp.xlsx
+++ b/temp.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Word</t>
   </si>
@@ -20,7 +20,16 @@
     <t>Count</t>
   </si>
   <si>
+    <t>tundra</t>
+  </si>
+  <si>
+    <t>temperature</t>
+  </si>
+  <si>
     <t>climate</t>
+  </si>
+  <si>
+    <t>animals</t>
   </si>
 </sst>
 </file>
@@ -37,7 +46,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <name val="Arial"/>
+      <name val="Lato"/>
       <sz val="16.0"/>
       <b val="true"/>
     </font>
@@ -51,12 +60,12 @@
     </fill>
     <fill>
       <patternFill patternType="none">
-        <fgColor indexed="48"/>
+        <fgColor indexed="42"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="48"/>
+        <fgColor indexed="42"/>
       </patternFill>
     </fill>
   </fills>
@@ -84,7 +93,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -107,7 +116,31 @@
         <v>2</v>
       </c>
       <c r="B3" t="n" s="2">
-        <v>14.0</v>
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" t="n" s="2">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" t="n" s="2">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" t="n" s="2">
+        <v>4.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>